<commit_message>
Changed models, fixed test data.
</commit_message>
<xml_diff>
--- a/tests/data/test_ilmoitukset/ilmoitukset.xlsx
+++ b/tests/data/test_ilmoitukset/ilmoitukset.xlsx
@@ -430,7 +430,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -460,11 +460,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -479,16 +474,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -544,7 +533,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -557,7 +546,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,11 +558,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -582,18 +579,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -723,8 +708,8 @@
   </sheetPr>
   <dimension ref="A1:BT5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BT12" activeCellId="0" sqref="BT12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BR1" activeCellId="0" sqref="BR:BR"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -740,8 +725,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="54.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="57.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="52" min="52" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="64" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="52" min="52" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="64" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="70" min="70" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -952,7 +938,7 @@
       <c r="BQ1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BR1" s="6" t="s">
         <v>69</v>
       </c>
       <c r="BS1" s="4" t="s">
@@ -984,7 +970,7 @@
       <c r="G2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -993,13 +979,13 @@
       <c r="J2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>75</v>
       </c>
       <c r="O2" s="1" t="s">
@@ -1011,7 +997,7 @@
       <c r="Q2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>81</v>
       </c>
       <c r="U2" s="7" t="s">
@@ -1020,55 +1006,55 @@
       <c r="V2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA2" s="1" t="n">
         <v>120</v>
       </c>
       <c r="AD2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AF2" s="0" t="s">
+      <c r="AF2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AG2" s="0" t="s">
+      <c r="AG2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AH2" s="0" t="s">
+      <c r="AH2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AI2" s="0" t="n">
+      <c r="AI2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AO2" s="0" t="s">
+      <c r="AO2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AP2" s="0" t="s">
+      <c r="AP2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AQ2" s="0" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AV2" s="0" t="n">
+      <c r="AV2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AW2" s="0" t="s">
+      <c r="AW2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AX2" s="0" t="s">
+      <c r="AX2" s="1" t="s">
         <v>76</v>
       </c>
       <c r="AY2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="AZ2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="BA2" s="0" t="s">
+      <c r="BA2" s="1" t="s">
         <v>81</v>
       </c>
       <c r="BB2" s="7" t="s">
@@ -1080,19 +1066,19 @@
       <c r="BD2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="BE2" s="0" t="s">
+      <c r="BE2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BF2" s="0" t="s">
+      <c r="BF2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BQ2" s="0" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BR2" s="0" t="s">
+      <c r="BR2" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="BT2" s="0" t="s">
+      <c r="BT2" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1118,7 +1104,7 @@
       <c r="G3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>79</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -1127,13 +1113,13 @@
       <c r="J3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>75</v>
       </c>
       <c r="O3" s="1" t="s">
@@ -1145,7 +1131,7 @@
       <c r="Q3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="1" t="s">
         <v>81</v>
       </c>
       <c r="U3" s="7" t="s">
@@ -1154,55 +1140,55 @@
       <c r="V3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="Z3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <v>120</v>
       </c>
       <c r="AD3" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AG3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AH3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AI3" s="0" t="n">
+      <c r="AI3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AO3" s="0" t="s">
+      <c r="AO3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AP3" s="0" t="s">
+      <c r="AP3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AQ3" s="0" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AV3" s="0" t="n">
+      <c r="AV3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AW3" s="0" t="s">
+      <c r="AW3" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="AX3" s="0" t="s">
+      <c r="AX3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="AY3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AZ3" s="3" t="s">
+      <c r="AZ3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="BA3" s="0" t="s">
+      <c r="BA3" s="1" t="s">
         <v>98</v>
       </c>
       <c r="BB3" s="7" t="s">
@@ -1214,19 +1200,19 @@
       <c r="BD3" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="BE3" s="0" t="s">
+      <c r="BE3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BF3" s="0" t="s">
+      <c r="BF3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BQ3" s="0" t="s">
+      <c r="BQ3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BR3" s="0" t="s">
+      <c r="BR3" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="BT3" s="0" t="s">
+      <c r="BT3" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1234,7 +1220,7 @@
       <c r="A4" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1249,7 +1235,7 @@
       <c r="F4" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="10" t="s">
         <v>106</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1261,10 +1247,10 @@
       <c r="J4" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>98</v>
       </c>
       <c r="P4" s="7" t="s">
@@ -1273,7 +1259,7 @@
       <c r="Q4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="R4" s="1" t="s">
         <v>98</v>
       </c>
       <c r="U4" s="7" t="s">
@@ -1282,70 +1268,70 @@
       <c r="V4" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="W4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="Z4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AA4" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="AD4" s="0" t="s">
+      <c r="AD4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AF4" s="0" t="s">
+      <c r="AF4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AG4" s="0" t="s">
+      <c r="AG4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AH4" s="0" t="s">
+      <c r="AH4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="AI4" s="0" t="n">
+      <c r="AI4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="AJ4" s="0" t="s">
+      <c r="AJ4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AK4" s="0" t="s">
+      <c r="AK4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AL4" s="0" t="s">
+      <c r="AL4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AM4" s="0" t="s">
+      <c r="AM4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AN4" s="0" t="s">
+      <c r="AN4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AO4" s="0" t="s">
+      <c r="AO4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AP4" s="0" t="s">
+      <c r="AP4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AQ4" s="0" t="s">
+      <c r="AQ4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AR4" s="0" t="s">
+      <c r="AR4" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AS4" s="0" t="s">
+      <c r="AS4" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AT4" s="0" t="s">
+      <c r="AT4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AU4" s="0" t="s">
+      <c r="AU4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AV4" s="0" t="n">
+      <c r="AV4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AX4" s="7" t="s">
@@ -1354,10 +1340,10 @@
       <c r="AY4" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="AZ4" s="3" t="s">
+      <c r="AZ4" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="BA4" s="0" t="s">
+      <c r="BA4" s="1" t="s">
         <v>98</v>
       </c>
       <c r="BB4" s="7" t="s">
@@ -1369,19 +1355,19 @@
       <c r="BD4" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="BE4" s="0" t="s">
+      <c r="BE4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BF4" s="0" t="s">
+      <c r="BF4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BQ4" s="0" t="s">
+      <c r="BQ4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BR4" s="10" t="s">
+      <c r="BR4" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="BT4" s="0" t="s">
+      <c r="BT4" s="1" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1404,7 +1390,7 @@
       <c r="F5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>128</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -1434,10 +1420,10 @@
       <c r="R5" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="S5" s="0" t="s">
+      <c r="S5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="T5" s="0" t="s">
+      <c r="T5" s="1" t="s">
         <v>132</v>
       </c>
       <c r="U5" s="7" t="s">
@@ -1446,85 +1432,85 @@
       <c r="V5" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="W5" s="0" t="s">
+      <c r="W5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="Y5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z5" s="0" t="n">
+      <c r="Z5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AA5" s="0" t="n">
+      <c r="AA5" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="AD5" s="0" t="s">
+      <c r="AD5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AF5" s="0" t="s">
+      <c r="AF5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AG5" s="0" t="s">
+      <c r="AG5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AH5" s="0" t="s">
+      <c r="AH5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="AI5" s="0" t="n">
+      <c r="AI5" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="AJ5" s="0" t="s">
+      <c r="AJ5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="AK5" s="0" t="s">
+      <c r="AK5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AL5" s="12" t="s">
+      <c r="AL5" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AM5" s="12" t="s">
+      <c r="AM5" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AN5" s="0" t="s">
+      <c r="AN5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AO5" s="0" t="s">
+      <c r="AO5" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AP5" s="0" t="s">
+      <c r="AP5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AQ5" s="12" t="s">
+      <c r="AQ5" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="AR5" s="0" t="s">
+      <c r="AR5" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AS5" s="0" t="s">
+      <c r="AS5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AT5" s="0" t="s">
+      <c r="AT5" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AU5" s="0" t="s">
+      <c r="AU5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AV5" s="0" t="n">
+      <c r="AV5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AW5" s="0" t="s">
+      <c r="AW5" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="AX5" s="0" t="s">
+      <c r="AX5" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AY5" s="0" t="s">
+      <c r="AY5" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AZ5" s="3" t="s">
+      <c r="AZ5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="BA5" s="0" t="s">
+      <c r="BA5" s="1" t="s">
         <v>131</v>
       </c>
       <c r="BB5" s="7" t="s">
@@ -1536,19 +1522,19 @@
       <c r="BD5" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="BE5" s="0" t="s">
+      <c r="BE5" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="BF5" s="0" t="s">
+      <c r="BF5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BQ5" s="0" t="s">
+      <c r="BQ5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="BR5" s="10" t="s">
+      <c r="BR5" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="BT5" s="0" t="s">
+      <c r="BT5" s="1" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>